<commit_message>
tercer avance guia importacion
</commit_message>
<xml_diff>
--- a/optimizacion/Guias/Importacion parametros/parametros.xlsx
+++ b/optimizacion/Guias/Importacion parametros/parametros.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanfeliperengifo/Desktop/optimizacion/optimizacion/Guias/Importacion parametros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB4B2D1-FE3E-B64E-BF4F-D291EE2AB3BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE8DA30-0DB8-4643-9B08-3623F8ACD4EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27740" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27740" windowHeight="15860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="pesoObjetos" sheetId="4" r:id="rId1"/>
-    <sheet name="pesoMaxExcursionistas" sheetId="5" r:id="rId2"/>
+    <sheet name="pesoObjetos" sheetId="5" r:id="rId1"/>
+    <sheet name="pesoMaxExcursionistas" sheetId="4" r:id="rId2"/>
     <sheet name="preferencias" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
@@ -250,11 +250,170 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="163442" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="CuadroTexto 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61AEB1CB-D0C4-1640-AF79-EBFE6985FA33}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2263140" y="160020"/>
+              <a:ext cx="163442" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="es-CO" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="es-CO" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝒑</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝒊</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-CO" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="CuadroTexto 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61AEB1CB-D0C4-1640-AF79-EBFE6985FA33}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2263140" y="160020"/>
+              <a:ext cx="163442" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝒑_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝒊</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-CO" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="161518" cy="172227"/>
+    <xdr:ext cx="163378" cy="185564"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -270,8 +429,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2567940" y="5303520"/>
-              <a:ext cx="161518" cy="172227"/>
+              <a:off x="2819400" y="190500"/>
+              <a:ext cx="163378" cy="185564"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -323,10 +482,10 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="es-CO" sz="1100" b="1" i="1">
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>𝒊</m:t>
+                          <m:t>𝒋</m:t>
                         </m:r>
                       </m:sub>
                     </m:sSub>
@@ -352,8 +511,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2567940" y="5303520"/>
-              <a:ext cx="161518" cy="172227"/>
+              <a:off x="2819400" y="190500"/>
+              <a:ext cx="163378" cy="185564"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -385,160 +544,13 @@
                 <a:rPr lang="es-CO" sz="1100" b="1" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝒃_𝒊</a:t>
+                <a:t>𝒃_</a:t>
               </a:r>
-              <a:endParaRPr lang="es-CO" sz="1100" b="1"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="165302" cy="185564"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="CuadroTexto 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61AEB1CB-D0C4-1640-AF79-EBFE6985FA33}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2796540" y="2827020"/>
-              <a:ext cx="165302" cy="185564"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="es-CO" sz="1100" b="1" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="es-CO" sz="1100" b="1" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝒑</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="es-CO" sz="1100" b="1" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝒋</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="es-CO" sz="1100" b="1"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="CuadroTexto 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61AEB1CB-D0C4-1640-AF79-EBFE6985FA33}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2796540" y="2827020"/>
-              <a:ext cx="165302" cy="185564"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
               <a:r>
-                <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝒑_𝒋</a:t>
+                <a:t>𝒋</a:t>
               </a:r>
               <a:endParaRPr lang="es-CO" sz="1100" b="1"/>
             </a:p>
@@ -561,8 +573,8 @@
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="201273" cy="185564"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -644,7 +656,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -966,11 +978,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496A1D5A-D45D-1C40-A90B-46E9952554C3}">
+  <dimension ref="B2:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B198F3-6A04-43BF-B184-6CC37F8CDA75}">
   <dimension ref="B2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1105,133 +1238,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496A1D5A-D45D-1C40-A90B-46E9952554C3}">
-  <dimension ref="B2:C14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="5">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>